<commit_message>
Sprint Backlog & Product Backlog
</commit_message>
<xml_diff>
--- a/deliverable3/Product_Backlog_RootDigital.xlsx
+++ b/deliverable3/Product_Backlog_RootDigital.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\colea\Documents\GitHub\Root-Digital\deliverable2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ewm25\Documents\GitHub\Root-Digital\deliverable3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DE7D30B-2BA7-4DAC-BB85-B5FC888C8D8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF25FDEA-210B-475F-9B9D-1F2678AD3DAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -453,18 +453,18 @@
   </sheetPr>
   <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.88671875" customWidth="1"/>
+    <col min="1" max="1" width="4.85546875" customWidth="1"/>
     <col min="2" max="2" width="59" style="7" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="21.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
@@ -484,7 +484,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -504,7 +504,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -524,7 +524,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -544,7 +544,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -564,7 +564,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -584,7 +584,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -604,7 +604,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -624,7 +624,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -644,7 +644,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -662,7 +662,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -682,7 +682,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -702,7 +702,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -722,7 +722,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -742,7 +742,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -762,7 +762,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -782,7 +782,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -802,7 +802,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -810,7 +810,7 @@
         <v>13</v>
       </c>
       <c r="C18" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>32</v>
@@ -822,7 +822,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" ht="63" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -842,7 +842,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -862,7 +862,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" ht="63" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -882,7 +882,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -902,7 +902,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" ht="63" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -922,7 +922,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -942,7 +942,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="5"/>
       <c r="C25" s="1"/>
@@ -950,7 +950,7 @@
       <c r="E25" s="1"/>
       <c r="F25" s="3"/>
     </row>
-    <row r="26" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="5"/>
       <c r="C26" s="1"/>
@@ -958,7 +958,7 @@
       <c r="E26" s="1"/>
       <c r="F26" s="3"/>
     </row>
-    <row r="27" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="5"/>
       <c r="C27" s="1"/>
@@ -966,7 +966,7 @@
       <c r="E27" s="1"/>
       <c r="F27" s="3"/>
     </row>
-    <row r="28" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="5"/>
       <c r="C28" s="1"/>
@@ -974,7 +974,7 @@
       <c r="E28" s="1"/>
       <c r="F28" s="3"/>
     </row>
-    <row r="29" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="5"/>
       <c r="C29" s="1"/>
@@ -982,7 +982,7 @@
       <c r="E29" s="1"/>
       <c r="F29" s="3"/>
     </row>
-    <row r="30" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="5"/>
       <c r="C30" s="1"/>
@@ -990,7 +990,7 @@
       <c r="E30" s="1"/>
       <c r="F30" s="3"/>
     </row>
-    <row r="31" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="5"/>
       <c r="C31" s="1"/>
@@ -998,7 +998,7 @@
       <c r="E31" s="1"/>
       <c r="F31" s="3"/>
     </row>
-    <row r="32" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="5"/>
       <c r="C32" s="1"/>
@@ -1006,7 +1006,7 @@
       <c r="E32" s="1"/>
       <c r="F32" s="3"/>
     </row>
-    <row r="33" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="5"/>
       <c r="C33" s="1"/>
@@ -1014,7 +1014,7 @@
       <c r="E33" s="1"/>
       <c r="F33" s="3"/>
     </row>
-    <row r="34" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="5"/>
       <c r="C34" s="1"/>
@@ -1022,7 +1022,7 @@
       <c r="E34" s="1"/>
       <c r="F34" s="3"/>
     </row>
-    <row r="35" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="5"/>
       <c r="C35" s="1"/>
@@ -1030,7 +1030,7 @@
       <c r="E35" s="1"/>
       <c r="F35" s="3"/>
     </row>
-    <row r="36" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="5"/>
       <c r="C36" s="1"/>
@@ -1038,7 +1038,7 @@
       <c r="E36" s="1"/>
       <c r="F36" s="3"/>
     </row>
-    <row r="37" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="5"/>
       <c r="C37" s="1"/>

</xml_diff>